<commit_message>
scratch notes and slides for rotation talk
</commit_message>
<xml_diff>
--- a/Summary/scratch_notes.xlsx
+++ b/Summary/scratch_notes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\GitHub\demo_for_ccgb\Summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEBD3D9-AB45-466F-8FFA-FB1D3DFFC5BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE8AC5D-92D5-4816-8B57-D0D4794E5A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
+    <workbookView xWindow="1896" yWindow="2820" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="25">
   <si>
     <t>theta</t>
   </si>
@@ -79,6 +80,36 @@
   </si>
   <si>
     <t>T_23 (scaled)</t>
+  </si>
+  <si>
+    <t>Theta</t>
+  </si>
+  <si>
+    <t>two_epoch</t>
+  </si>
+  <si>
+    <t>exponential</t>
+  </si>
+  <si>
+    <t>bottleneck</t>
+  </si>
+  <si>
+    <t>three_epoch</t>
+  </si>
+  <si>
+    <t>p_copri</t>
+  </si>
+  <si>
+    <t>o_splanchnicus</t>
+  </si>
+  <si>
+    <t>a_shahii</t>
+  </si>
+  <si>
+    <t>coprococcus_sp</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -433,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD05AD1F-39C1-48D3-93E8-7D0B7093A3C0}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1240,4 +1271,1078 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A941B0-2F65-4D9C-86F5-1774512E76E7}">
+  <dimension ref="A1:K47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>2026.6041198099999</v>
+      </c>
+      <c r="G3">
+        <v>6851.08948573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1.49516307</v>
+      </c>
+      <c r="G4">
+        <v>3.9692834100000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0.44708505999999998</v>
+      </c>
+      <c r="G6">
+        <v>0.39557179999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>B3/4*1000000000</f>
+        <v>506651029952.5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:K8" si="0">C3/4*1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1712772371432.5</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>B8/B4</f>
+        <v>338860048190.26196</v>
+      </c>
+      <c r="C9" t="e">
+        <f t="shared" ref="C9:K9" si="1">C8/C4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>431506696427.22742</v>
+      </c>
+      <c r="H9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>2*B6*B9</f>
+        <v>302998529953.49231</v>
+      </c>
+      <c r="C10" t="e">
+        <f t="shared" ref="C10:K10" si="2">2*C6*C9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>341383761235.54382</v>
+      </c>
+      <c r="H10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <f>2*B7*B9</f>
+        <v>0</v>
+      </c>
+      <c r="C11" t="e">
+        <f t="shared" ref="C11:K11" si="3">2*C7*C9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1939.1988649299999</v>
+      </c>
+      <c r="G15">
+        <v>6651.9430162500003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>1.62764391</v>
+      </c>
+      <c r="G16">
+        <v>5.5207001800000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>1.09100781</v>
+      </c>
+      <c r="G18">
+        <v>0.65275521000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
+        <f>B15/4*1000000000</f>
+        <v>484799716232.5</v>
+      </c>
+      <c r="C20">
+        <f t="shared" ref="C20:K20" si="4">C15/4*1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="4"/>
+        <v>1662985754062.5</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <f>B20/B16</f>
+        <v>297853672571.72363</v>
+      </c>
+      <c r="C21" t="e">
+        <f t="shared" ref="C21" si="5">C20/C16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D21" t="e">
+        <f t="shared" ref="D21" si="6">D20/D16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E21" t="e">
+        <f t="shared" ref="E21" si="7">E20/E16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F21" t="e">
+        <f t="shared" ref="F21" si="8">F20/F16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21">
+        <f>G20/G16</f>
+        <v>301227326216.16486</v>
+      </c>
+      <c r="H21" t="e">
+        <f>H20/H16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I21" t="e">
+        <f t="shared" ref="I21" si="9">I20/I16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J21" t="e">
+        <f t="shared" ref="J21" si="10">J20/J16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" t="e">
+        <f t="shared" ref="K21" si="11">K20/K16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <f>2*B18*B21</f>
+        <v>649921366025.86658</v>
+      </c>
+      <c r="C22" t="e">
+        <f t="shared" ref="C22" si="12">2*C18*C21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D22" t="e">
+        <f t="shared" ref="D22" si="13">2*D18*D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E22" t="e">
+        <f t="shared" ref="E22" si="14">2*E18*E21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F22" t="e">
+        <f t="shared" ref="F22" si="15">2*F18*F21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22">
+        <f>2*G18*G21</f>
+        <v>393255413163.94238</v>
+      </c>
+      <c r="H22" t="e">
+        <f>2*H18*H21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I22" t="e">
+        <f t="shared" ref="I22" si="16">2*I18*I21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J22" t="e">
+        <f t="shared" ref="J22" si="17">2*J18*J21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" t="e">
+        <f t="shared" ref="K22" si="18">2*K18*K21</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <f>2*B19*B21</f>
+        <v>0</v>
+      </c>
+      <c r="C23" t="e">
+        <f t="shared" ref="C23:K23" si="19">2*C19*C21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>1931.3930001599999</v>
+      </c>
+      <c r="G27">
+        <v>6649.6250826400001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>1.07053664</v>
+      </c>
+      <c r="G28">
+        <v>1.00120516</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>1.6312748500000001</v>
+      </c>
+      <c r="G29">
+        <v>5.5203546100000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30">
+        <v>0.98098777000000004</v>
+      </c>
+      <c r="G30">
+        <v>0.65317188000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <f>B27/4*1000000000</f>
+        <v>482848250040</v>
+      </c>
+      <c r="C32">
+        <f t="shared" ref="C32:K32" si="20">C27/4*1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="20"/>
+        <v>1662406270660</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33">
+        <f>B32/B28</f>
+        <v>451033838542.88257</v>
+      </c>
+      <c r="C33" t="e">
+        <f t="shared" ref="C33" si="21">C32/C28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D33" t="e">
+        <f t="shared" ref="D33" si="22">D32/D28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E33" t="e">
+        <f t="shared" ref="E33" si="23">E32/E28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F33" t="e">
+        <f t="shared" ref="F33" si="24">F32/F28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33" si="25">G32/G28</f>
+        <v>1660405216709.0308</v>
+      </c>
+      <c r="H33" t="e">
+        <f t="shared" ref="H33" si="26">H32/H28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I33" t="e">
+        <f t="shared" ref="I33" si="27">I32/I28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J33" t="e">
+        <f t="shared" ref="J33" si="28">J32/J28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K33" t="e">
+        <f t="shared" ref="K33" si="29">K32/K28</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34">
+        <f>2*B30*B33</f>
+        <v>884917358933.44482</v>
+      </c>
+      <c r="C34" t="e">
+        <f t="shared" ref="C34" si="30">2*C30*C33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D34" t="e">
+        <f t="shared" ref="D34" si="31">2*D30*D33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E34" t="e">
+        <f t="shared" ref="E34" si="32">2*E30*E33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F34" t="e">
+        <f t="shared" ref="F34" si="33">2*F30*F33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ref="G34" si="34">2*G30*G33</f>
+        <v>2169059993919.2903</v>
+      </c>
+      <c r="H34" t="e">
+        <f t="shared" ref="H34" si="35">2*H30*H33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I34" t="e">
+        <f t="shared" ref="I34" si="36">2*I30*I33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J34" t="e">
+        <f t="shared" ref="J34" si="37">2*J30*J33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K34" t="e">
+        <f t="shared" ref="K34" si="38">2*K30*K33</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" t="e">
+        <f>2*B31*B33</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C35" t="e">
+        <f t="shared" ref="C35:K35" si="39">2*C31*C33</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G35" t="e">
+        <f t="shared" si="39"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" t="e">
+        <f t="shared" si="39"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
+      <c r="J38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39">
+        <v>2028.0812273500001</v>
+      </c>
+      <c r="G39">
+        <v>6405.0042083099997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>2.64925027</v>
+      </c>
+      <c r="G40">
+        <v>1.69793265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41">
+        <v>1.49440752</v>
+      </c>
+      <c r="G41">
+        <v>4.91266537</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>6.31432E-3</v>
+      </c>
+      <c r="G42">
+        <v>0.46533746999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43">
+        <v>0.43254745</v>
+      </c>
+      <c r="G43">
+        <v>0.27208793999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <f>B39/4*1000000000</f>
+        <v>507020306837.5</v>
+      </c>
+      <c r="C44">
+        <f t="shared" ref="C44:K44" si="40">C39/4*1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="40"/>
+        <v>1601251052077.5</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <f>B44/B40</f>
+        <v>191382563051.50815</v>
+      </c>
+      <c r="C45" t="e">
+        <f t="shared" ref="C45" si="41">C44/C40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D45" t="e">
+        <f t="shared" ref="D45" si="42">D44/D40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E45" t="e">
+        <f t="shared" ref="E45" si="43">E44/E40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F45" t="e">
+        <f t="shared" ref="F45" si="44">F44/F40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ref="G45" si="45">G44/G40</f>
+        <v>943059226805.90417</v>
+      </c>
+      <c r="H45" t="e">
+        <f t="shared" ref="H45" si="46">H44/H40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I45" t="e">
+        <f t="shared" ref="I45" si="47">I44/I40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J45" t="e">
+        <f t="shared" ref="J45" si="48">J44/J40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K45" t="e">
+        <f t="shared" ref="K45" si="49">K44/K40</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46">
+        <f>2*B42*B45</f>
+        <v>2416901491.0547976</v>
+      </c>
+      <c r="C46" t="e">
+        <f t="shared" ref="C46" si="50">2*C42*C45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D46" t="e">
+        <f t="shared" ref="D46" si="51">2*D42*D45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E46" t="e">
+        <f t="shared" ref="E46" si="52">2*E42*E45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F46" t="e">
+        <f t="shared" ref="F46" si="53">2*F42*F45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ref="G46" si="54">2*G42*G45</f>
+        <v>877681589324.03125</v>
+      </c>
+      <c r="H46" t="e">
+        <f t="shared" ref="H46" si="55">2*H42*H45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I46" t="e">
+        <f t="shared" ref="I46" si="56">2*I42*I45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J46" t="e">
+        <f t="shared" ref="J46" si="57">2*J42*J45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" t="e">
+        <f t="shared" ref="K46" si="58">2*K42*K45</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47">
+        <f>2*B43*B45</f>
+        <v>165564079244.78815</v>
+      </c>
+      <c r="C47" t="e">
+        <f t="shared" ref="C47:K47" si="59">2*C43*C45</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="59"/>
+        <v>513190084639.22241</v>
+      </c>
+      <c r="H47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" t="e">
+        <f t="shared" si="59"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
analysis for lab meeting.
</commit_message>
<xml_diff>
--- a/Summary/scratch_notes.xlsx
+++ b/Summary/scratch_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\GitHub\demo_for_ccgb\Summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE8AC5D-92D5-4816-8B57-D0D4794E5A2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D712BE6-FE7E-4CE1-88E6-0B3D4768DA32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1896" yWindow="2820" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="26">
   <si>
     <t>theta</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>exp_time (years)</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,13 +1278,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A941B0-2F65-4D9C-86F5-1774512E76E7}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1324,8 +1330,29 @@
       <c r="B3">
         <v>2026.6041198099999</v>
       </c>
+      <c r="C3">
+        <v>1147.0820226400001</v>
+      </c>
+      <c r="D3">
+        <v>470.10972137300001</v>
+      </c>
+      <c r="E3">
+        <v>976.51368738899998</v>
+      </c>
+      <c r="F3">
+        <v>6313.92536406</v>
+      </c>
       <c r="G3">
         <v>6851.08948573</v>
+      </c>
+      <c r="H3">
+        <v>2411.6673514399999</v>
+      </c>
+      <c r="I3">
+        <v>3541.16650011</v>
+      </c>
+      <c r="J3">
+        <v>212.26033721300001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -1335,14 +1362,62 @@
       <c r="B4">
         <v>1.49516307</v>
       </c>
+      <c r="C4">
+        <v>12.624995520000001</v>
+      </c>
+      <c r="D4">
+        <v>12.859820320000001</v>
+      </c>
+      <c r="E4">
+        <v>2.8063426200000001</v>
+      </c>
+      <c r="F4">
+        <v>2.1856705000000001</v>
+      </c>
       <c r="G4">
         <v>3.9692834100000001</v>
+      </c>
+      <c r="H4">
+        <v>1.27668903</v>
+      </c>
+      <c r="I4">
+        <v>3.8038503499999998</v>
+      </c>
+      <c r="J4">
+        <v>25.942298539999999</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1351,38 +1426,86 @@
       <c r="B6">
         <v>0.44708505999999998</v>
       </c>
+      <c r="C6">
+        <v>18.011779730000001</v>
+      </c>
+      <c r="D6">
+        <v>5.2635385899999996</v>
+      </c>
+      <c r="E6">
+        <v>2.1535067400000001</v>
+      </c>
+      <c r="F6">
+        <v>1.56531566</v>
+      </c>
       <c r="G6">
         <v>0.39557179999999997</v>
+      </c>
+      <c r="H6">
+        <v>1.5076925800000001</v>
+      </c>
+      <c r="I6">
+        <v>7.0481710000000003E-2</v>
+      </c>
+      <c r="J6">
+        <v>28.369623050000001</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <f>B3/4*1000000000</f>
-        <v>506651029952.5</v>
+        <f>B3/4/0.000000001</f>
+        <v>506651029952.49994</v>
       </c>
       <c r="C8">
         <f t="shared" ref="C8:K8" si="0">C3/4*1000000000</f>
-        <v>0</v>
+        <v>286770505660</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>117527430343.25</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>244128421847.25</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1578481341015</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -1390,15 +1513,15 @@
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>602916837860</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>885291625027.5</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>53065084303.25</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
@@ -1411,39 +1534,39 @@
       </c>
       <c r="B9">
         <f>B8/B4</f>
-        <v>338860048190.26196</v>
-      </c>
-      <c r="C9" t="e">
+        <v>338860048190.2619</v>
+      </c>
+      <c r="C9">
         <f t="shared" ref="C9:K9" si="1">C8/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" t="e">
+        <v>22714503558.097103</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E9" t="e">
+        <v>9139119164.8663712</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" t="e">
+        <v>86991666700.785797</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>722195473203.76062</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
         <v>431506696427.22742</v>
       </c>
-      <c r="H9" t="e">
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I9" t="e">
+        <v>472250347337.91046</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" t="e">
+        <v>232735660862.02631</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>2045504341.9313762</v>
       </c>
       <c r="K9" t="e">
         <f t="shared" si="1"/>
@@ -1456,39 +1579,39 @@
       </c>
       <c r="B10">
         <f>2*B6*B9</f>
-        <v>302998529953.49231</v>
-      </c>
-      <c r="C10" t="e">
+        <v>302998529953.49225</v>
+      </c>
+      <c r="C10">
         <f t="shared" ref="C10:K10" si="2">2*C6*C9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" t="e">
+        <v>818257269529.49255</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E10" t="e">
+        <v>96208212805.765427</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" t="e">
+        <v>374674281127.9516</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>2260927767573.9136</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
         <v>341383761235.54382</v>
       </c>
-      <c r="H10" t="e">
+      <c r="H10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I10" t="e">
+        <v>1424016689167.5808</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" t="e">
+        <v>32807214711.071377</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>116060374255.46291</v>
       </c>
       <c r="K10" t="e">
         <f t="shared" si="2"/>
@@ -1499,845 +1622,1331 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="e">
         <f>2*B7*B9</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C11" t="e">
         <f t="shared" ref="C11:K11" si="3">2*C7*C9</f>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D11" t="e">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E11" t="e">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="F11" t="e">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G11">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" t="e">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H11" t="e">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I11" t="e">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="J11" t="e">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="K11" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <f>B10/3650</f>
+        <v>83013295.877669111</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:K12" si="4">C10/3650</f>
+        <v>224180073.84369659</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="4"/>
+        <v>26358414.467332993</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
+        <v>102650487.98026071</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>619432265.08874345</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="4"/>
+        <v>93529797.598779127</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>390141558.67604953</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="4"/>
+        <v>8988278.0030332543</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>31797362.809715863</v>
+      </c>
+      <c r="K12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>5</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>20</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H15" t="s">
         <v>21</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I15" t="s">
         <v>22</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>1939.1988649299999</v>
-      </c>
-      <c r="G15">
-        <v>6651.9430162500003</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>1.62764391</v>
+        <v>1939.1988649299999</v>
+      </c>
+      <c r="C16">
+        <v>1514.8694253399999</v>
+      </c>
+      <c r="D16">
+        <v>173.19143288699999</v>
+      </c>
+      <c r="E16">
+        <v>437.65990236800002</v>
+      </c>
+      <c r="F16">
+        <v>1986.0456640899999</v>
       </c>
       <c r="G16">
-        <v>5.5207001800000004</v>
+        <v>6651.9430162500003</v>
+      </c>
+      <c r="H16">
+        <v>2458.3802003300002</v>
+      </c>
+      <c r="I16">
+        <v>3539.1473797600001</v>
+      </c>
+      <c r="J16">
+        <v>1738.3802492499999</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>1.62764391</v>
+      </c>
+      <c r="C17">
+        <v>2.0241613200000002</v>
+      </c>
+      <c r="D17">
+        <v>11.614573910000001</v>
+      </c>
+      <c r="E17">
+        <v>6.6955190099999999</v>
+      </c>
+      <c r="F17">
+        <v>7.3102929200000002</v>
+      </c>
+      <c r="G17">
+        <v>5.5207001800000004</v>
+      </c>
+      <c r="H17">
+        <v>1.2597083600000001</v>
+      </c>
+      <c r="I17">
+        <v>5.1329904500000003</v>
+      </c>
+      <c r="J17">
+        <v>3.5467534299999999</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>1.09100781</v>
-      </c>
-      <c r="G18">
-        <v>0.65275521000000003</v>
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>1.09100781</v>
+      </c>
+      <c r="C19">
+        <v>3.17342171</v>
+      </c>
+      <c r="D19">
+        <v>4.3999589200000004</v>
+      </c>
+      <c r="E19">
+        <v>17.296584490000001</v>
+      </c>
+      <c r="F19">
+        <v>25.361710779999999</v>
+      </c>
+      <c r="G19">
+        <v>0.65275521000000003</v>
+      </c>
+      <c r="H19">
+        <v>3.4824461599999998</v>
+      </c>
+      <c r="I19">
+        <v>9.8380969999999998E-2</v>
+      </c>
+      <c r="J19">
+        <v>4.6332282100000004</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <f>B15/4*1000000000</f>
-        <v>484799716232.5</v>
-      </c>
-      <c r="C20">
-        <f t="shared" ref="C20:K20" si="4">C15/4*1000000000</f>
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>1662985754062.5</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <f>B20/B16</f>
-        <v>297853672571.72363</v>
-      </c>
-      <c r="C21" t="e">
-        <f t="shared" ref="C21" si="5">C20/C16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" t="e">
-        <f t="shared" ref="D21" si="6">D20/D16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E21" t="e">
-        <f t="shared" ref="E21" si="7">E20/E16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F21" t="e">
-        <f t="shared" ref="F21" si="8">F20/F16</f>
-        <v>#DIV/0!</v>
+        <f>B16/4*1000000000</f>
+        <v>484799716232.5</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:K21" si="5">C16/4*1000000000</f>
+        <v>378717356335</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="5"/>
+        <v>43297858221.75</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="5"/>
+        <v>109414975592</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="5"/>
+        <v>496511416022.5</v>
       </c>
       <c r="G21">
-        <f>G20/G16</f>
-        <v>301227326216.16486</v>
-      </c>
-      <c r="H21" t="e">
-        <f>H20/H16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I21" t="e">
-        <f t="shared" ref="I21" si="9">I20/I16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J21" t="e">
-        <f t="shared" ref="J21" si="10">J20/J16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" t="e">
-        <f t="shared" ref="K21" si="11">K20/K16</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="5"/>
+        <v>1662985754062.5</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="5"/>
+        <v>614595050082.5</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>884786844940</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>434595062312.5</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B22">
-        <f>2*B18*B21</f>
-        <v>649921366025.86658</v>
-      </c>
-      <c r="C22" t="e">
-        <f t="shared" ref="C22" si="12">2*C18*C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D22" t="e">
-        <f t="shared" ref="D22" si="13">2*D18*D21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E22" t="e">
-        <f t="shared" ref="E22" si="14">2*E18*E21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F22" t="e">
-        <f t="shared" ref="F22" si="15">2*F18*F21</f>
-        <v>#DIV/0!</v>
+        <f>B21/B17</f>
+        <v>297853672571.72363</v>
+      </c>
+      <c r="C22">
+        <f t="shared" ref="C22" si="6">C21/C17</f>
+        <v>187098405938.81122</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22" si="7">D21/D17</f>
+        <v>3727890369.2257786</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22" si="8">E21/E17</f>
+        <v>16341522655.46327</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22" si="9">F21/F17</f>
+        <v>67919496722.779747</v>
       </c>
       <c r="G22">
-        <f>2*G18*G21</f>
-        <v>393255413163.94238</v>
-      </c>
-      <c r="H22" t="e">
-        <f>2*H18*H21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I22" t="e">
-        <f t="shared" ref="I22" si="16">2*I18*I21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J22" t="e">
-        <f t="shared" ref="J22" si="17">2*J18*J21</f>
-        <v>#DIV/0!</v>
+        <f>G21/G17</f>
+        <v>301227326216.16486</v>
+      </c>
+      <c r="H22">
+        <f>H21/H17</f>
+        <v>487886775699.81354</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22" si="10">I21/I17</f>
+        <v>172372587394.93661</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22" si="11">J21/J17</f>
+        <v>122533204207.68579</v>
       </c>
       <c r="K22" t="e">
-        <f t="shared" ref="K22" si="18">2*K18*K21</f>
+        <f t="shared" ref="K22" si="12">K21/K17</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23">
+        <f>2*B19*B22</f>
+        <v>649921366025.86658</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23" si="13">2*C19*C22</f>
+        <v>1187484286625.2329</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ref="D23" si="14">2*D19*D22</f>
+        <v>32805128965.714119</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23" si="15">2*E19*E22</f>
+        <v>565305054610.93921</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23" si="16">2*F19*F22</f>
+        <v>3445109264412.5952</v>
+      </c>
+      <c r="G23">
+        <f>2*G19*G22</f>
+        <v>393255413163.94238</v>
+      </c>
+      <c r="H23">
+        <f>2*H19*H22</f>
+        <v>3398078857101.1938</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ref="I23" si="17">2*I19*I22</f>
+        <v>33916364698.647274</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ref="J23" si="18">2*J19*J22</f>
+        <v>1135448596793.4812</v>
+      </c>
+      <c r="K23" t="e">
+        <f t="shared" ref="K23" si="19">2*K19*K22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>14</v>
       </c>
-      <c r="B23">
-        <f>2*B19*B21</f>
-        <v>0</v>
-      </c>
-      <c r="C23" t="e">
-        <f t="shared" ref="C23:K23" si="19">2*C19*C21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F23" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-      <c r="H23" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I23" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J23" t="e">
-        <f t="shared" si="19"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K23" t="e">
-        <f t="shared" si="19"/>
+      <c r="B24" t="e">
+        <f>2*B20*B22</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C24" t="e">
+        <f t="shared" ref="C24:K24" si="20">2*C20*C22</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J24" t="e">
+        <f t="shared" si="20"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" t="e">
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" t="s">
-        <v>21</v>
-      </c>
-      <c r="I26" t="s">
-        <v>22</v>
-      </c>
-      <c r="J26" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <f>B23/3650</f>
+        <v>178060648.2262648</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:K25" si="21">C23/3650</f>
+        <v>325338160.71924192</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="21"/>
+        <v>8987706.5659490731</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="21"/>
+        <v>154878097.15368196</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="21"/>
+        <v>943865551.89386165</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="21"/>
+        <v>107741209.08601162</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="21"/>
+        <v>930980508.79484761</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="21"/>
+        <v>9292154.7119581569</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="21"/>
+        <v>311081807.34067976</v>
+      </c>
+      <c r="K25" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <v>1931.3930001599999</v>
-      </c>
-      <c r="G27">
-        <v>6649.6250826400001</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28">
-        <v>1.07053664</v>
-      </c>
-      <c r="G28">
-        <v>1.00120516</v>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B29">
-        <v>1.6312748500000001</v>
+        <v>1931.3930001599999</v>
+      </c>
+      <c r="C29">
+        <v>1435.9800853199999</v>
+      </c>
+      <c r="D29">
+        <v>902.972409954</v>
+      </c>
+      <c r="E29">
+        <v>1263.6996722199999</v>
+      </c>
+      <c r="F29">
+        <v>6979.7591718000003</v>
       </c>
       <c r="G29">
-        <v>5.5203546100000001</v>
+        <v>6649.6250826400001</v>
+      </c>
+      <c r="H29">
+        <v>2267.7693192299998</v>
+      </c>
+      <c r="I29">
+        <v>3636.75605937</v>
+      </c>
+      <c r="J29">
+        <v>2279.2085805699999</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>0.98098777000000004</v>
+        <v>1.07053664</v>
+      </c>
+      <c r="C30">
+        <v>2.24845827</v>
+      </c>
+      <c r="D30">
+        <v>59.815547680000002</v>
+      </c>
+      <c r="E30">
+        <v>1.39324194</v>
+      </c>
+      <c r="F30">
+        <v>1.98581751</v>
       </c>
       <c r="G30">
-        <v>0.65317188000000004</v>
+        <v>1.00120516</v>
+      </c>
+      <c r="H30">
+        <v>2.7205513400000001</v>
+      </c>
+      <c r="I30">
+        <v>0.46397566000000001</v>
+      </c>
+      <c r="J30">
+        <v>5.7221805200000002</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-      <c r="G31" t="s">
-        <v>24</v>
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>1.6312748500000001</v>
+      </c>
+      <c r="C31">
+        <v>1.7991231599999999</v>
+      </c>
+      <c r="D31">
+        <v>3.5711893199999998</v>
+      </c>
+      <c r="E31">
+        <v>2.3096104</v>
+      </c>
+      <c r="F31">
+        <v>1.9825688400000001</v>
+      </c>
+      <c r="G31">
+        <v>5.5203546100000001</v>
+      </c>
+      <c r="H31">
+        <v>1.16513409</v>
+      </c>
+      <c r="I31">
+        <v>4.4183940799999997</v>
+      </c>
+      <c r="J31">
+        <v>1.95484218</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B32">
-        <f>B27/4*1000000000</f>
-        <v>482848250040</v>
+        <v>0.98098777000000004</v>
       </c>
       <c r="C32">
-        <f t="shared" ref="C32:K32" si="20">C27/4*1000000000</f>
-        <v>0</v>
+        <v>1.2397629100000001</v>
       </c>
       <c r="D32">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.59972168</v>
       </c>
       <c r="E32">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.68463977</v>
       </c>
       <c r="F32">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.2225338100000001</v>
       </c>
       <c r="G32">
-        <f t="shared" si="20"/>
-        <v>1662406270660</v>
+        <v>0.65317188000000004</v>
       </c>
       <c r="H32">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.89676621999999995</v>
       </c>
       <c r="I32">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>0.17523284</v>
       </c>
       <c r="J32">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.1557514600000001</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33">
-        <f>B32/B28</f>
-        <v>451033838542.88257</v>
-      </c>
-      <c r="C33" t="e">
-        <f t="shared" ref="C33" si="21">C32/C28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" t="e">
-        <f t="shared" ref="D33" si="22">D32/D28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" t="e">
-        <f t="shared" ref="E33" si="23">E32/E28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F33" t="e">
-        <f t="shared" ref="F33" si="24">F32/F28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G33">
-        <f t="shared" ref="G33" si="25">G32/G28</f>
-        <v>1660405216709.0308</v>
-      </c>
-      <c r="H33" t="e">
-        <f t="shared" ref="H33" si="26">H32/H28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I33" t="e">
-        <f t="shared" ref="I33" si="27">I32/I28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J33" t="e">
-        <f t="shared" ref="J33" si="28">J32/J28</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K33" t="e">
-        <f t="shared" ref="K33" si="29">K32/K28</f>
-        <v>#DIV/0!</v>
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B34">
-        <f>2*B30*B33</f>
-        <v>884917358933.44482</v>
-      </c>
-      <c r="C34" t="e">
-        <f t="shared" ref="C34" si="30">2*C30*C33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" t="e">
-        <f t="shared" ref="D34" si="31">2*D30*D33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" t="e">
-        <f t="shared" ref="E34" si="32">2*E30*E33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F34" t="e">
-        <f t="shared" ref="F34" si="33">2*F30*F33</f>
-        <v>#DIV/0!</v>
+        <f>B29/4*1000000000</f>
+        <v>482848250040</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:K34" si="22">C29/4*1000000000</f>
+        <v>358995021330</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="22"/>
+        <v>225743102488.5</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="22"/>
+        <v>315924918055</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="22"/>
+        <v>1744939792950</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34" si="34">2*G30*G33</f>
-        <v>2169059993919.2903</v>
-      </c>
-      <c r="H34" t="e">
-        <f t="shared" ref="H34" si="35">2*H30*H33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I34" t="e">
-        <f t="shared" ref="I34" si="36">2*I30*I33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J34" t="e">
-        <f t="shared" ref="J34" si="37">2*J30*J33</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K34" t="e">
-        <f t="shared" ref="K34" si="38">2*K30*K33</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="22"/>
+        <v>1662406270660</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="22"/>
+        <v>566942329807.5</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="22"/>
+        <v>909189014842.5</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="22"/>
+        <v>569802145142.5</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="22"/>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" t="e">
-        <f>2*B31*B33</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C35" t="e">
-        <f t="shared" ref="C35:K35" si="39">2*C31*C33</f>
+        <v>8</v>
+      </c>
+      <c r="B35">
+        <f>B34/B30</f>
+        <v>451033838542.88257</v>
+      </c>
+      <c r="C35">
+        <f t="shared" ref="C35" si="23">C34/C30</f>
+        <v>159662745855.63022</v>
+      </c>
+      <c r="D35">
+        <f t="shared" ref="D35" si="24">D34/D30</f>
+        <v>3773987052.6000338</v>
+      </c>
+      <c r="E35">
+        <f t="shared" ref="E35" si="25">E34/E30</f>
+        <v>226755245434.97449</v>
+      </c>
+      <c r="F35">
+        <f t="shared" ref="F35" si="26">F34/F30</f>
+        <v>878700980408.81921</v>
+      </c>
+      <c r="G35">
+        <f t="shared" ref="G35" si="27">G34/G30</f>
+        <v>1660405216709.0308</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35" si="28">H34/H30</f>
+        <v>208392439235.31323</v>
+      </c>
+      <c r="I35">
+        <f t="shared" ref="I35" si="29">I34/I30</f>
+        <v>1959561876246.9133</v>
+      </c>
+      <c r="J35">
+        <f t="shared" ref="J35" si="30">J34/J30</f>
+        <v>99577799608.199005</v>
+      </c>
+      <c r="K35" t="e">
+        <f t="shared" ref="K35" si="31">K34/K30</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D35" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E35" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F35" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G35" t="e">
-        <f t="shared" si="39"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H35" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I35" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J35" t="e">
-        <f t="shared" si="39"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K35" t="e">
-        <f t="shared" si="39"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36">
+        <f>2*B32*B35</f>
+        <v>884917358933.44482</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36" si="32">2*C32*C35</f>
+        <v>395887900841.13312</v>
+      </c>
+      <c r="D36">
+        <f t="shared" ref="D36" si="33">2*D32*D35</f>
+        <v>12074657816.167149</v>
+      </c>
+      <c r="E36">
+        <f t="shared" ref="E36" si="34">2*E32*E35</f>
+        <v>764001809031.73792</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36" si="35">2*F32*F35</f>
+        <v>2148483314859.8584</v>
+      </c>
+      <c r="G36">
+        <f t="shared" ref="G36" si="36">2*G32*G35</f>
+        <v>2169059993919.2903</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36" si="37">2*H32*H35</f>
+        <v>373758600019.26306</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36" si="38">2*I32*I35</f>
+        <v>686759185460.95032</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ref="J36" si="39">2*J32*J35</f>
+        <v>230174374561.52686</v>
+      </c>
+      <c r="K36" t="e">
+        <f t="shared" ref="K36" si="40">2*K32*K35</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B37" t="e">
+        <f>2*B33*B35</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C37" t="e">
+        <f t="shared" ref="C37:K37" si="41">2*C33*C35</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J37" t="e">
+        <f t="shared" si="41"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K37" t="e">
+        <f t="shared" si="41"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>2</v>
-      </c>
-      <c r="D38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" t="s">
-        <v>5</v>
-      </c>
-      <c r="G38" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" t="s">
-        <v>21</v>
-      </c>
-      <c r="I38" t="s">
-        <v>22</v>
-      </c>
-      <c r="J38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39">
-        <v>2028.0812273500001</v>
-      </c>
-      <c r="G39">
-        <v>6405.0042083099997</v>
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <f>B36/3650</f>
+        <v>242443112.03656024</v>
+      </c>
+      <c r="C38">
+        <f t="shared" ref="C38:K38" si="42">C36/3650</f>
+        <v>108462438.58661181</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="42"/>
+        <v>3308125.4290868901</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="42"/>
+        <v>209315564.11828437</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="42"/>
+        <v>588625565.71502972</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="42"/>
+        <v>594263012.0326823</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="42"/>
+        <v>102399616.44363372</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="42"/>
+        <v>188153201.49615076</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="42"/>
+        <v>63061472.482610099</v>
+      </c>
+      <c r="K38" t="e">
+        <f t="shared" si="42"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40">
-        <v>2.64925027</v>
-      </c>
-      <c r="G40">
-        <v>1.69793265</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41">
-        <v>1.49440752</v>
-      </c>
-      <c r="G41">
-        <v>4.91266537</v>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I41" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B42">
-        <v>6.31432E-3</v>
+        <v>2028.0812273500001</v>
+      </c>
+      <c r="C42">
+        <v>1586.49500784</v>
+      </c>
+      <c r="D42">
+        <v>451.06789978400002</v>
+      </c>
+      <c r="E42">
+        <v>4235.6442018400003</v>
+      </c>
+      <c r="F42">
+        <v>1460.26124873</v>
       </c>
       <c r="G42">
-        <v>0.46533746999999998</v>
+        <v>6405.0042083099997</v>
+      </c>
+      <c r="H42">
+        <v>2248.5797190100002</v>
+      </c>
+      <c r="J42">
+        <v>807.30313363799996</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B43">
-        <v>0.43254745</v>
+        <v>2.64925027</v>
+      </c>
+      <c r="C43">
+        <v>3.2435803299999999</v>
+      </c>
+      <c r="D43">
+        <v>10.317690689999999</v>
+      </c>
+      <c r="E43">
+        <v>0.13057176000000001</v>
+      </c>
+      <c r="F43">
+        <v>5.6729456899999997</v>
       </c>
       <c r="G43">
-        <v>0.27208793999999997</v>
+        <v>1.69793265</v>
+      </c>
+      <c r="H43">
+        <v>2.8722564500000001</v>
+      </c>
+      <c r="J43">
+        <v>24.066358080000001</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B44">
-        <f>B39/4*1000000000</f>
-        <v>507020306837.5</v>
+        <v>1.49440752</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:K44" si="40">C39/4*1000000000</f>
-        <v>0</v>
+        <v>1.73262388</v>
       </c>
       <c r="D44">
-        <f t="shared" si="40"/>
-        <v>0</v>
+        <v>12.075340069999999</v>
       </c>
       <c r="E44">
-        <f t="shared" si="40"/>
-        <v>0</v>
+        <v>0.64729155000000005</v>
       </c>
       <c r="F44">
-        <f t="shared" si="40"/>
-        <v>0</v>
+        <v>9.4331015800000007</v>
       </c>
       <c r="G44">
-        <f t="shared" si="40"/>
-        <v>1601251052077.5</v>
+        <v>4.91266537</v>
       </c>
       <c r="H44">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1.22885559</v>
       </c>
       <c r="J44">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="40"/>
-        <v>0</v>
+        <v>4.6316497400000003</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B45">
-        <f>B44/B40</f>
-        <v>191382563051.50815</v>
-      </c>
-      <c r="C45" t="e">
-        <f t="shared" ref="C45" si="41">C44/C40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D45" t="e">
-        <f t="shared" ref="D45" si="42">D44/D40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E45" t="e">
-        <f t="shared" ref="E45" si="43">E44/E40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F45" t="e">
-        <f t="shared" ref="F45" si="44">F44/F40</f>
-        <v>#DIV/0!</v>
+        <v>6.31432E-3</v>
+      </c>
+      <c r="C45">
+        <v>0.40179331000000001</v>
+      </c>
+      <c r="D45">
+        <v>0.90845072000000004</v>
+      </c>
+      <c r="E45">
+        <v>0.29392339000000001</v>
+      </c>
+      <c r="F45">
+        <v>5.84565073</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G45" si="45">G44/G40</f>
-        <v>943059226805.90417</v>
-      </c>
-      <c r="H45" t="e">
-        <f t="shared" ref="H45" si="46">H44/H40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I45" t="e">
-        <f t="shared" ref="I45" si="47">I44/I40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J45" t="e">
-        <f t="shared" ref="J45" si="48">J44/J40</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K45" t="e">
-        <f t="shared" ref="K45" si="49">K44/K40</f>
-        <v>#DIV/0!</v>
+        <v>0.46533746999999998</v>
+      </c>
+      <c r="H45">
+        <v>0.49102278999999999</v>
+      </c>
+      <c r="J45">
+        <v>4.1497465199999999</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B46">
-        <f>2*B42*B45</f>
-        <v>2416901491.0547976</v>
-      </c>
-      <c r="C46" t="e">
-        <f t="shared" ref="C46" si="50">2*C42*C45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D46" t="e">
-        <f t="shared" ref="D46" si="51">2*D42*D45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E46" t="e">
-        <f t="shared" ref="E46" si="52">2*E42*E45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46" t="e">
-        <f t="shared" ref="F46" si="53">2*F42*F45</f>
-        <v>#DIV/0!</v>
+        <v>0.43254745</v>
+      </c>
+      <c r="C46">
+        <v>0.54790132000000002</v>
+      </c>
+      <c r="D46">
+        <v>3.75907656</v>
+      </c>
+      <c r="E46">
+        <v>0.50844703999999996</v>
+      </c>
+      <c r="F46">
+        <v>7.3622157499999998</v>
       </c>
       <c r="G46">
-        <f t="shared" ref="G46" si="54">2*G42*G45</f>
-        <v>877681589324.03125</v>
-      </c>
-      <c r="H46" t="e">
-        <f t="shared" ref="H46" si="55">2*H42*H45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I46" t="e">
-        <f t="shared" ref="I46" si="56">2*I42*I45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J46" t="e">
-        <f t="shared" ref="J46" si="57">2*J42*J45</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K46" t="e">
-        <f t="shared" ref="K46" si="58">2*K42*K45</f>
-        <v>#DIV/0!</v>
+        <v>0.27208793999999997</v>
+      </c>
+      <c r="H46">
+        <v>0.33065141999999997</v>
+      </c>
+      <c r="J46">
+        <v>1.3229835599999999</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <f>B42/4*1000000000</f>
+        <v>507020306837.5</v>
+      </c>
+      <c r="C47">
+        <f t="shared" ref="C47:K47" si="43">C42/4*1000000000</f>
+        <v>396623751960</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="43"/>
+        <v>112766974946</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="43"/>
+        <v>1058911050460.0001</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="43"/>
+        <v>365065312182.5</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="43"/>
+        <v>1601251052077.5</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="43"/>
+        <v>562144929752.5</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="43"/>
+        <v>201825783409.5</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <f>B47/B43</f>
+        <v>191382563051.50815</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48" si="44">C47/C43</f>
+        <v>122279614379.08954</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48" si="45">D47/D43</f>
+        <v>10929478149.145796</v>
+      </c>
+      <c r="E48">
+        <f t="shared" ref="E48" si="46">E47/E43</f>
+        <v>8109801464420.791</v>
+      </c>
+      <c r="F48">
+        <f t="shared" ref="F48" si="47">F47/F43</f>
+        <v>64351984336.113045</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ref="G48" si="48">G47/G43</f>
+        <v>943059226805.90417</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48" si="49">H47/H43</f>
+        <v>195715438206.25766</v>
+      </c>
+      <c r="I48" t="e">
+        <f t="shared" ref="I48" si="50">I47/I43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J48">
+        <f t="shared" ref="J48" si="51">J47/J43</f>
+        <v>8386220413.5167589</v>
+      </c>
+      <c r="K48" t="e">
+        <f t="shared" ref="K48" si="52">K47/K43</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49">
+        <f>2*B45*B48</f>
+        <v>2416901491.0547976</v>
+      </c>
+      <c r="C49">
+        <f t="shared" ref="C49" si="53">2*C45*C48</f>
+        <v>98262262013.795959</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ref="D49" si="54">2*D45*D48</f>
+        <v>19857784587.631531</v>
+      </c>
+      <c r="E49">
+        <f t="shared" ref="E49" si="55">2*E45*E48</f>
+        <v>4767320677299.0469</v>
+      </c>
+      <c r="F49">
+        <f t="shared" ref="F49" si="56">2*F45*F48</f>
+        <v>752358448422.69556</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ref="G49" si="57">2*G45*G48</f>
+        <v>877681589324.03125</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ref="H49" si="58">2*H45*H48</f>
+        <v>192201481028.21844</v>
+      </c>
+      <c r="I49" t="e">
+        <f t="shared" ref="I49" si="59">2*I45*I48</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ref="J49" si="60">2*J45*J48</f>
+        <v>69601377953.88826</v>
+      </c>
+      <c r="K49" t="e">
+        <f t="shared" ref="K49" si="61">2*K45*K48</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>14</v>
       </c>
-      <c r="B47">
-        <f>2*B43*B45</f>
+      <c r="B50">
+        <f>2*B46*B48</f>
         <v>165564079244.78815</v>
       </c>
-      <c r="C47" t="e">
-        <f t="shared" ref="C47:K47" si="59">2*C43*C45</f>
+      <c r="C50">
+        <f t="shared" ref="C50:K50" si="62">2*C46*C48</f>
+        <v>133994324254.78828</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="62"/>
+        <v>82169490246.97229</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="62"/>
+        <v>8246809099144.832</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="62"/>
+        <v>947546385246.16943</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="62"/>
+        <v>513190084639.22241</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="62"/>
+        <v>129427175117.64268</v>
+      </c>
+      <c r="I50" t="e">
+        <f t="shared" si="62"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D47" t="e">
-        <f t="shared" si="59"/>
+      <c r="J50">
+        <f t="shared" si="62"/>
+        <v>22189663475.238148</v>
+      </c>
+      <c r="K50" t="e">
+        <f t="shared" si="62"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="E47" t="e">
-        <f t="shared" si="59"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <f>B49/3650</f>
+        <v>662164.79206980753</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:K51" si="63">C49/3650</f>
+        <v>26921167.675012592</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="63"/>
+        <v>5440488.928118228</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="63"/>
+        <v>1306115254.0545335</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="63"/>
+        <v>206125602.30758783</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="63"/>
+        <v>240460709.40384418</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="63"/>
+        <v>52657940.00773108</v>
+      </c>
+      <c r="I51" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F47" t="e">
-        <f t="shared" si="59"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="59"/>
-        <v>513190084639.22241</v>
-      </c>
-      <c r="H47" t="e">
-        <f t="shared" si="59"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I47" t="e">
-        <f t="shared" si="59"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J47" t="e">
-        <f t="shared" si="59"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K47" t="e">
-        <f t="shared" si="59"/>
+      <c r="J51">
+        <f t="shared" si="63"/>
+        <v>19068870.672298152</v>
+      </c>
+      <c r="K51" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
slides for meeting 2/14/2022
</commit_message>
<xml_diff>
--- a/Summary/scratch_notes.xlsx
+++ b/Summary/scratch_notes.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\GitHub\demo_for_ccgb\Summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5261b2f2f3e51194/Desktop/GitHub/demo_for_ccgb/Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D712BE6-FE7E-4CE1-88E6-0B3D4768DA32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{2D712BE6-FE7E-4CE1-88E6-0B3D4768DA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFE54740-B41D-4A96-B022-581CF62E1D99}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
+    <workbookView xWindow="-14385" yWindow="5070" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="35">
   <si>
     <t>theta</t>
   </si>
@@ -114,6 +115,33 @@
   <si>
     <t>exp_time (years)</t>
   </si>
+  <si>
+    <t>a_finegoldii</t>
+  </si>
+  <si>
+    <t>a_muciniphila</t>
+  </si>
+  <si>
+    <t>b_bacterium</t>
+  </si>
+  <si>
+    <t>b_intestinihominis</t>
+  </si>
+  <si>
+    <t>b_thetaiotamicron</t>
+  </si>
+  <si>
+    <t>p_distasonis</t>
+  </si>
+  <si>
+    <t>p_merdae</t>
+  </si>
+  <si>
+    <t>p_sp</t>
+  </si>
+  <si>
+    <t>bottlegrowth</t>
+  </si>
 </sst>
 </file>
 
@@ -148,9 +176,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -467,20 +496,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD05AD1F-39C1-48D3-93E8-7D0B7093A3C0}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.85546875" style="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="8.88671875" style="1"/>
+    <col min="4" max="8" width="8.85546875" style="1"/>
     <col min="9" max="9" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +535,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -539,7 +568,7 @@
         <v>484379654186.20044</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -572,7 +601,7 @@
         <v>409887463579.13208</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -605,7 +634,7 @@
         <v>530.77426597640317</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -638,7 +667,7 @@
         <v>293985784609.99835</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -671,7 +700,7 @@
         <v>1464459854724.179</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -730,7 +759,7 @@
         <v>27059691400.22588</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -763,7 +792,7 @@
         <v>234416473455.68375</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
@@ -796,7 +825,7 @@
         <v>76748343007.349243</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -829,7 +858,7 @@
         <v>17620856.129667666</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -862,7 +891,7 @@
         <v>655817759642.96606</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
@@ -894,7 +923,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
@@ -934,7 +963,7 @@
         <v>10008680027.759027</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -974,7 +1003,7 @@
         <v>280787564628.04163</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -1014,7 +1043,7 @@
         <v>204100822389.98944</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1083,7 @@
         <v>97892749242.20369</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1094,7 +1123,7 @@
         <v>21423600300948.473</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1149,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1150,7 +1179,7 @@
         <v>150503672165.8494</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1209,7 @@
         <v>454481851607.41315</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
@@ -1210,7 +1239,7 @@
         <v>26816669260.97868</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1240,7 +1269,7 @@
         <v>32143976526.896801</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
@@ -1280,21 +1309,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A941B0-2F65-4D9C-86F5-1774512E76E7}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K51" sqref="K2:K51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1322,8 +1351,11 @@
       <c r="J2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1354,8 +1386,11 @@
       <c r="J3">
         <v>212.26033721300001</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>10999.521090800001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1386,8 +1421,11 @@
       <c r="J4">
         <v>25.942298539999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K4" s="1">
+        <v>0.10011102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1419,7 +1457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1450,8 +1488,11 @@
       <c r="J6">
         <v>28.369623050000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <v>6.0414825199999998E-7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1483,7 +1524,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1525,10 +1566,10 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2749880272700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1568,12 +1609,12 @@
         <f t="shared" si="1"/>
         <v>2045504341.9313762</v>
       </c>
-      <c r="K9" t="e">
+      <c r="K9">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>27468307412111.074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1613,12 +1654,12 @@
         <f t="shared" si="2"/>
         <v>116060374255.46291</v>
       </c>
-      <c r="K10" t="e">
+      <c r="K10">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>33189859.816851098</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1658,12 +1699,12 @@
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K11" t="e">
+      <c r="K11">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1703,17 +1744,17 @@
         <f t="shared" si="4"/>
         <v>31797362.809715863</v>
       </c>
-      <c r="K12" t="e">
+      <c r="K12">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>9093.1122785893422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -1742,7 +1783,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1773,8 +1814,11 @@
       <c r="J16">
         <v>1738.3802492499999</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>10999.521210700001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1805,8 +1849,11 @@
       <c r="J17">
         <v>3.5467534299999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K17" s="1">
+        <v>0.10712925700000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1838,7 +1885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1869,8 +1916,11 @@
       <c r="J19">
         <v>4.6332282100000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K19" s="1">
+        <v>9.5599966699999999E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>13</v>
       </c>
@@ -1902,7 +1952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1944,10 +1994,10 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2749880302675</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1987,12 +2037,12 @@
         <f t="shared" ref="J22" si="11">J21/J17</f>
         <v>122533204207.68579</v>
       </c>
-      <c r="K22" t="e">
+      <c r="K22">
         <f t="shared" ref="K22" si="12">K21/K17</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>25668807753189.215</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -2032,12 +2082,12 @@
         <f t="shared" ref="J23" si="18">2*J19*J22</f>
         <v>1135448596793.4812</v>
       </c>
-      <c r="K23" t="e">
+      <c r="K23">
         <f t="shared" ref="K23" si="19">2*K19*K22</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>49078743.328671813</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -2077,12 +2127,12 @@
         <f t="shared" si="20"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K24" t="e">
+      <c r="K24">
         <f t="shared" si="20"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2122,17 +2172,17 @@
         <f t="shared" si="21"/>
         <v>311081807.34067976</v>
       </c>
-      <c r="K25" t="e">
+      <c r="K25">
         <f t="shared" si="21"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>13446.231048951182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>1</v>
       </c>
@@ -2161,7 +2211,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2192,8 +2242,11 @@
       <c r="J29">
         <v>2279.2085805699999</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>10999.5212161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -2224,8 +2277,11 @@
       <c r="J30">
         <v>5.7221805200000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K30" s="1">
+        <v>9.0705826200000006E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -2256,8 +2312,11 @@
       <c r="J31">
         <v>1.95484218</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K31" s="1">
+        <v>7.1635162700000005E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -2288,8 +2347,11 @@
       <c r="J32">
         <v>1.1557514600000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K32" s="1">
+        <v>8.1182600800000001E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -2321,7 +2383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -2363,10 +2425,10 @@
       </c>
       <c r="K34">
         <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2749880304025</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2406,12 +2468,12 @@
         <f t="shared" ref="J35" si="30">J34/J30</f>
         <v>99577799608.199005</v>
       </c>
-      <c r="K35" t="e">
+      <c r="K35">
         <f t="shared" ref="K35" si="31">K34/K30</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+        <v>30316468293466.688</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -2451,12 +2513,12 @@
         <f t="shared" ref="J36" si="39">2*J32*J35</f>
         <v>230174374561.52686</v>
       </c>
-      <c r="K36" t="e">
+      <c r="K36">
         <f t="shared" ref="K36" si="40">2*K32*K35</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+        <v>49223394.862687267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2496,12 +2558,12 @@
         <f t="shared" si="41"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K37" t="e">
+      <c r="K37">
         <f t="shared" si="41"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>25</v>
       </c>
@@ -2541,17 +2603,17 @@
         <f t="shared" si="42"/>
         <v>63061472.482610099</v>
       </c>
-      <c r="K38" t="e">
+      <c r="K38">
         <f t="shared" si="42"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+        <v>13485.861606215689</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>1</v>
       </c>
@@ -2580,7 +2642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>15</v>
       </c>
@@ -2608,8 +2670,11 @@
       <c r="J42">
         <v>807.30313363799996</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K42" s="1">
+        <v>11433.249814700001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -2637,8 +2702,11 @@
       <c r="J43">
         <v>24.066358080000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K43" s="1">
+        <v>0.106804355</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -2666,8 +2734,11 @@
       <c r="J44">
         <v>4.6316497400000003</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K44" s="1">
+        <v>2.3367373400000001E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2695,8 +2766,11 @@
       <c r="J45">
         <v>4.1497465199999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K45" s="1">
+        <v>5.5860816100000001E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -2724,8 +2798,11 @@
       <c r="J46">
         <v>1.3229835599999999</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K46" s="1">
+        <v>1.0382691999999999E-6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -2767,10 +2844,10 @@
       </c>
       <c r="K47">
         <f t="shared" si="43"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2858312453675</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2810,12 +2887,12 @@
         <f t="shared" ref="J48" si="51">J47/J43</f>
         <v>8386220413.5167589</v>
       </c>
-      <c r="K48" t="e">
+      <c r="K48">
         <f t="shared" ref="K48" si="52">K47/K43</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+        <v>26762133938030.898</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2855,12 +2932,12 @@
         <f t="shared" ref="J49" si="60">2*J45*J48</f>
         <v>69601377953.88826</v>
       </c>
-      <c r="K49" t="e">
+      <c r="K49">
         <f t="shared" ref="K49" si="61">2*K45*K48</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2989909284.7118258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
@@ -2900,42 +2977,42 @@
         <f t="shared" si="62"/>
         <v>22189663475.238148</v>
       </c>
-      <c r="K50" t="e">
+      <c r="K50">
         <f t="shared" si="62"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+        <v>55572598.788264379</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>25</v>
       </c>
       <c r="B51">
-        <f>B49/3650</f>
-        <v>662164.79206980753</v>
+        <f>B50/3650</f>
+        <v>45360021.710900865</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:K51" si="63">C49/3650</f>
-        <v>26921167.675012592</v>
+        <f t="shared" ref="C51:K51" si="63">C50/3650</f>
+        <v>36710773.768435143</v>
       </c>
       <c r="D51">
         <f t="shared" si="63"/>
-        <v>5440488.928118228</v>
+        <v>22512189.10875953</v>
       </c>
       <c r="E51">
         <f t="shared" si="63"/>
-        <v>1306115254.0545335</v>
+        <v>2259399753.1903648</v>
       </c>
       <c r="F51">
         <f t="shared" si="63"/>
-        <v>206125602.30758783</v>
+        <v>259601749.38251218</v>
       </c>
       <c r="G51">
         <f t="shared" si="63"/>
-        <v>240460709.40384418</v>
+        <v>140600023.18882805</v>
       </c>
       <c r="H51">
         <f t="shared" si="63"/>
-        <v>52657940.00773108</v>
+        <v>35459500.032230869</v>
       </c>
       <c r="I51" t="e">
         <f t="shared" si="63"/>
@@ -2943,15 +3020,865 @@
       </c>
       <c r="J51">
         <f t="shared" si="63"/>
-        <v>19068870.672298152</v>
-      </c>
-      <c r="K51" t="e">
+        <v>6079359.8562296294</v>
+      </c>
+      <c r="K51">
         <f t="shared" si="63"/>
-        <v>#DIV/0!</v>
+        <v>15225.369531031336</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAF7C00-AE0C-4F81-A2C8-D740FFBB95E8}">
+  <dimension ref="A1:N51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S44" sqref="S44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>6489.6433083600004</v>
+      </c>
+      <c r="C3">
+        <v>7902.40041604</v>
+      </c>
+      <c r="D3">
+        <v>2529.8943693199999</v>
+      </c>
+      <c r="E3">
+        <v>4948.31021255</v>
+      </c>
+      <c r="F3">
+        <v>11359.4173157</v>
+      </c>
+      <c r="G3">
+        <v>11365.679670899999</v>
+      </c>
+      <c r="H3">
+        <v>10083.5247623</v>
+      </c>
+      <c r="I3">
+        <v>5609.0477814799997</v>
+      </c>
+      <c r="J3">
+        <v>4111.3837677600004</v>
+      </c>
+      <c r="M3">
+        <v>10999.521090800001</v>
+      </c>
+      <c r="N3">
+        <v>11156.912795800001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>1.9485699999999999E-3</v>
+      </c>
+      <c r="C4">
+        <v>4.5122599999999997E-3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.75243355199999995</v>
+      </c>
+      <c r="E4">
+        <v>3.0161699999999999E-3</v>
+      </c>
+      <c r="F4">
+        <v>4.2281200000000001E-3</v>
+      </c>
+      <c r="G4">
+        <v>8.1578399999999995E-3</v>
+      </c>
+      <c r="H4">
+        <v>6.2658599999999998E-3</v>
+      </c>
+      <c r="I4">
+        <v>6.5453000000000004E-3</v>
+      </c>
+      <c r="J4">
+        <v>3.6933399999999998E-3</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.10011102</v>
+      </c>
+      <c r="N4" s="1">
+        <v>3.6687242299999999E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>2.1031000000000001E-4</v>
+      </c>
+      <c r="C6">
+        <v>3.6393999999999999E-4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.1304600000000001E-6</v>
+      </c>
+      <c r="E6">
+        <v>1.6234999999999999E-4</v>
+      </c>
+      <c r="F6">
+        <v>3.7804000000000001E-4</v>
+      </c>
+      <c r="G6">
+        <v>1.7354E-4</v>
+      </c>
+      <c r="H6">
+        <v>2.5085999999999999E-4</v>
+      </c>
+      <c r="I6">
+        <v>2.5982000000000002E-4</v>
+      </c>
+      <c r="J6">
+        <v>2.0678E-4</v>
+      </c>
+      <c r="M6" s="1">
+        <v>6.0414825199999998E-7</v>
+      </c>
+      <c r="N6" s="1">
+        <v>2.2112685200000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>B3/4/0.000000001</f>
+        <v>1622410827090</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:K8" si="0">C3/4*1000000000</f>
+        <v>1975600104010</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>632473592330</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1237077553137.5</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>2839854328925</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2841419917725</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>2520881190575</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>1402261945370</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1027845941940.0001</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:N8" si="1">M3/4*1000000000</f>
+        <v>2749880272700</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8" si="2">N3/4*1000000000</f>
+        <v>2789228198950</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>B8/B4</f>
+        <v>832616137521361.88</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:K9" si="3">C8/C4</f>
+        <v>437829403449712.56</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="3"/>
+        <v>840570693118.16125</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>410148484050136.44</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>671658876504214.63</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>348305423705907.44</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>402320063099877.75</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>214239522309137.84</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>278297135367986.75</v>
+      </c>
+      <c r="K9" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:N9" si="4">M8/M4</f>
+        <v>27468307412111.074</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9" si="5">N8/N4</f>
+        <v>760271970332858.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <f>2*B6*B9/10000</f>
+        <v>35021499.976423524</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:J10" si="6">2*C6*C9/10000</f>
+        <v>31868726.618297674</v>
+      </c>
+      <c r="D10" s="1">
+        <f>2*D6*D9</f>
+        <v>5262745.8639573585</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="6"/>
+        <v>13317521.277107928</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="6"/>
+        <v>50782784.334730655</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="6"/>
+        <v>12088984.645984635</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>20185202.205847066</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="6"/>
+        <v>11132742.53727204</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>11509256.33027846</v>
+      </c>
+      <c r="K10" t="e">
+        <f t="shared" ref="K10" si="7">2*K6*K9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ref="M10:N10" si="8">2*M6*M9</f>
+        <v>33189859.816851098</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10" si="9">2*N6*N9</f>
+        <v>33623309492.708492</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="e">
+        <f>2*B7*B9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C11" t="e">
+        <f t="shared" ref="C11:K11" si="10">2*C7*C9</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J11" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K11" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11:N11" si="11">2*M7*M9</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11" si="12">2*N7*N9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2">
+        <f>B10/3650</f>
+        <v>9594.9315003900065</v>
+      </c>
+      <c r="C12" s="2">
+        <f t="shared" ref="C12:K12" si="13">C10/3650</f>
+        <v>8731.1579776158014</v>
+      </c>
+      <c r="D12" s="2">
+        <f>D10/365</f>
+        <v>14418.481819061257</v>
+      </c>
+      <c r="E12" s="2">
+        <f>E10/730</f>
+        <v>18243.179831654696</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="13"/>
+        <v>13913.091598556344</v>
+      </c>
+      <c r="G12" s="2">
+        <f>G10/730</f>
+        <v>16560.25293970498</v>
+      </c>
+      <c r="H12" s="2">
+        <f>H10/1825</f>
+        <v>11060.384770327159</v>
+      </c>
+      <c r="I12" s="2">
+        <f>I10/1210</f>
+        <v>9200.6136671669756</v>
+      </c>
+      <c r="J12" s="2">
+        <f>J10/730</f>
+        <v>15766.104562025288</v>
+      </c>
+      <c r="K12" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ref="M12:N12" si="14">M10/3650</f>
+        <v>9093.1122785893422</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12" si="15">N10/3650</f>
+        <v>9211865.6144406833</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M16">
+        <v>10999.521210700001</v>
+      </c>
+      <c r="N16">
+        <v>11141.287666099999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.10712925700000001</v>
+      </c>
+      <c r="N17" s="1">
+        <v>3.6692164700000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="M19" s="1">
+        <v>9.5599966699999999E-7</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2.3908978000000001E-5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ref="M21:N21" si="16">M16/4*1000000000</f>
+        <v>2749880302675</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="16"/>
+        <v>2785321916525</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ref="M22:N22" si="17">M21/M17</f>
+        <v>25668807753189.215</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="17"/>
+        <v>759105367398778.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:N23" si="18">2*M19*M22</f>
+        <v>49078743.328671813</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="18"/>
+        <v>36298867057.638641</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ref="M24:N24" si="19">2*M20*M22</f>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ref="M25:N25" si="20">M23/3650</f>
+        <v>13446.231048951182</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="20"/>
+        <v>9944895.0842845589</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="M29">
+        <v>10999.5212161</v>
+      </c>
+      <c r="N29">
+        <v>11147.4953621</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="M30" s="1">
+        <v>9.0705826200000006E-2</v>
+      </c>
+      <c r="N30" s="1">
+        <v>5.6314810599999996E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="1">
+        <v>7.1635162700000005E-2</v>
+      </c>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" s="1">
+        <v>8.1182600800000001E-7</v>
+      </c>
+      <c r="N32" s="1">
+        <v>2.9680548900000001E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ref="M34:N34" si="21">M29/4*1000000000</f>
+        <v>2749880304025</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="21"/>
+        <v>2786873840525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ref="M35:N35" si="22">M34/M30</f>
+        <v>30316468293466.688</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="22"/>
+        <v>494874050153513.31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36">
+        <f t="shared" ref="M36:N36" si="23">2*M32*M35</f>
+        <v>49223394.862687267</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="23"/>
+        <v>29376266889.84481</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ref="M37:N37" si="24">2*M33*M35</f>
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ref="M38:N38" si="25">M36/3650</f>
+        <v>13485.861606215689</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="25"/>
+        <v>8048292.2985876193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="M42" s="1">
+        <v>11433.249814700001</v>
+      </c>
+      <c r="N42">
+        <v>11157.8008329</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0.106804355</v>
+      </c>
+      <c r="N43" s="1">
+        <v>3.5754167199999998E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="M44" s="1">
+        <v>2.3367373400000001E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="M45" s="1">
+        <v>5.5860816100000001E-5</v>
+      </c>
+      <c r="N45" s="1">
+        <v>2.0934820700000001E-5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="M46" s="1">
+        <v>1.0382691999999999E-6</v>
+      </c>
+      <c r="N46" s="1">
+        <v>2.0934820700000001E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="M47">
+        <f t="shared" ref="M47:N47" si="26">M42/4*1000000000</f>
+        <v>2858312453675</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="26"/>
+        <v>2789450208225</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="M48">
+        <f t="shared" ref="M48:N48" si="27">M47/M43</f>
+        <v>26762133938030.898</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="27"/>
+        <v>780174851401657.13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="M49">
+        <f t="shared" ref="M49:N49" si="28">2*M45*M48</f>
+        <v>2989909284.7118258</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="28"/>
+        <v>32665641257.485672</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="M50">
+        <f t="shared" ref="M50:N50" si="29">2*M46*M48</f>
+        <v>55572598.788264379</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="29"/>
+        <v>32665641257.485672</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51">
+        <f t="shared" ref="M51:N51" si="30">M50/3650</f>
+        <v>15225.369531031336</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="30"/>
+        <v>8949490.7554755267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
merge, update rho_vs_mu script.
</commit_message>
<xml_diff>
--- a/Summary/scratch_notes.xlsx
+++ b/Summary/scratch_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5261b2f2f3e51194/Desktop/GitHub/demo_for_ccgb/Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{2D712BE6-FE7E-4CE1-88E6-0B3D4768DA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFE54740-B41D-4A96-B022-581CF62E1D99}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="13_ncr:1_{2D712BE6-FE7E-4CE1-88E6-0B3D4768DA32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB0A30B-EE9D-4FA7-A81D-546766D31C91}"/>
   <bookViews>
-    <workbookView xWindow="-14385" yWindow="5070" windowWidth="28800" windowHeight="11385" activeTab="2" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
+    <workbookView xWindow="0" yWindow="2235" windowWidth="15375" windowHeight="8325" activeTab="2" xr2:uid="{9F4B9699-7361-44C9-88F2-01D9ADA6A85E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1309,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A941B0-2F65-4D9C-86F5-1774512E76E7}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K51" sqref="K2:K51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3037,8 +3037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAAF7C00-AE0C-4F81-A2C8-D740FFBB95E8}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S44" sqref="S44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,7 +3306,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:N8" si="1">M3/4*1000000000</f>
+        <f t="shared" ref="M8" si="1">M3/4*1000000000</f>
         <v>2749880272700</v>
       </c>
       <c r="N8">
@@ -3359,7 +3359,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:N9" si="4">M8/M4</f>
+        <f t="shared" ref="M9" si="4">M8/M4</f>
         <v>27468307412111.074</v>
       </c>
       <c r="N9">
@@ -3412,7 +3412,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:N10" si="8">2*M6*M9</f>
+        <f t="shared" ref="M10" si="8">2*M6*M9</f>
         <v>33189859.816851098</v>
       </c>
       <c r="N10">
@@ -3465,7 +3465,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:N11" si="11">2*M7*M9</f>
+        <f t="shared" ref="M11" si="11">2*M7*M9</f>
         <v>0</v>
       </c>
       <c r="N11">
@@ -3518,7 +3518,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:N12" si="14">M10/3650</f>
+        <f t="shared" ref="M12" si="14">M10/3650</f>
         <v>9093.1122785893422</v>
       </c>
       <c r="N12">

</xml_diff>